<commit_message>
Major change to project EPIC definition
</commit_message>
<xml_diff>
--- a/_3 Develop/Design Calculations.xlsx
+++ b/_3 Develop/Design Calculations.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AllenProjects\PM_Folder\_3 Develop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\PWC 8D Elevate OLS\OLS Level Test Project\_Project Management\_3 Develop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0964801A-3E67-4BFC-BE6D-C80D10C3E2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DAB779-2577-44ED-B15C-55FD304428F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="200" windowWidth="17550" windowHeight="11280" xr2:uid="{2C504F31-A930-42E4-806E-D82B5918461B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11520" activeTab="1" xr2:uid="{2C504F31-A930-42E4-806E-D82B5918461B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tank" sheetId="1" r:id="rId1"/>
@@ -253,7 +253,7 @@
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
     <numFmt numFmtId="168" formatCode="0.0"/>
-    <numFmt numFmtId="172" formatCode="0.0000"/>
+    <numFmt numFmtId="169" formatCode="0.0000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -377,7 +377,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -918,7 +918,7 @@
                 <c:order val="5"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tank!$H$11</c15:sqref>
@@ -944,7 +944,7 @@
                 </c:spPr>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tank!$A$12:$A$18</c15:sqref>
@@ -980,7 +980,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tank!$H$12:$H$18</c15:sqref>
@@ -1015,7 +1015,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000013-240A-4813-BF1D-6E3B9128DB24}"/>
                   </c:ext>
@@ -1913,7 +1913,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-371B-4A1A-8917-7DBBA3FA224E}"/>
                   </c:ext>
@@ -4320,16 +4320,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>412750</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>374650</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>107950</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4395,15 +4395,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4988,25 +4988,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1CC6128-03DC-4EA5-BA09-5B0E87270B26}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H20" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" customWidth="1"/>
-    <col min="3" max="3" width="13.1796875" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" customWidth="1"/>
-    <col min="5" max="5" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -5014,7 +5014,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -5022,7 +5022,7 @@
         <v>8.4499999999999993</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -5030,7 +5030,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -5039,7 +5039,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -5047,7 +5047,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>31</v>
       </c>
@@ -5061,7 +5061,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="18"/>
       <c r="D10" s="16" t="s">
@@ -5089,7 +5089,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>59</v>
       </c>
@@ -5142,7 +5142,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>100</v>
       </c>
@@ -5199,7 +5199,7 @@
         <v>2.2204112554112556</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>75</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>1.7024372294372294</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>50</v>
       </c>
@@ -5313,7 +5313,7 @@
         <v>1.1405670995670996</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>25</v>
       </c>
@@ -5370,7 +5370,7 @@
         <v>0.5823549783549784</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5427,7 +5427,7 @@
         <v>0.32556277056277055</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5</v>
       </c>
@@ -5484,7 +5484,7 @@
         <v>8.5597402597402603E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>4</v>
       </c>
@@ -5541,7 +5541,7 @@
         <v>4.3164502164502162E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>45720</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -5563,12 +5563,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -5576,7 +5576,7 @@
         <v>-0.99299999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -5584,7 +5584,7 @@
         <v>9.6029999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -5593,7 +5593,7 @@
         <v>6.3639693506492234E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -5604,7 +5604,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>48</v>
       </c>
@@ -5616,7 +5616,7 @@
         <v>2.7832745999999995</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -5628,7 +5628,7 @@
         <v>2.8050212999999991</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B29" s="20" t="s">
         <v>50</v>
       </c>
@@ -5637,7 +5637,7 @@
         <v>2.1746699999999564E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>51</v>
       </c>
@@ -5657,22 +5657,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FBC02A7-3940-454D-9F05-4E2571E54D79}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7265625" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5680,7 +5680,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -5688,7 +5688,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -5696,7 +5696,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -5705,7 +5705,7 @@
         <v>20999.999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -5713,7 +5713,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -5722,7 +5722,7 @@
         <v>14.666666666666668</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -5730,7 +5730,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -5739,7 +5739,7 @@
         <v>1636.3636363636363</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -5747,7 +5747,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -5756,7 +5756,7 @@
         <v>20.533333333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -5774,10 +5774,10 @@
         <v>0.48701298701298695</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>12</v>
       </c>
@@ -5785,7 +5785,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -5793,7 +5793,7 @@
         <v>110000</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -5802,7 +5802,7 @@
         <v>99099.099099099098</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -5811,7 +5811,7 @@
         <v>104384.38438438441</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -5820,7 +5820,7 @@
         <v>214384.38438438441</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>17</v>
       </c>
@@ -5828,7 +5828,7 @@
         <v>104700</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -5836,7 +5836,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -5844,7 +5844,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -5856,7 +5856,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -5865,7 +5865,7 @@
         <v>14.659828562014544</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>23</v>
       </c>

</xml_diff>